<commit_message>
Revert "Merge branch 'master' of https://github.com/zhangnianli/BRFS"
This reverts commit de009babfc0421c454c57fddcfba3df67384f5f2, reversing
changes made to 85290850a1966d0c6c6765a87e3015ec82ca5886.
</commit_message>
<xml_diff>
--- a/doc/文件系统数据编码.xlsx
+++ b/doc/文件系统数据编码.xlsx
@@ -14,8 +14,77 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="F37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>校验方法</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>:
+0:crc</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1,2,3:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>保留</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>FID组成</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +209,10 @@
   </si>
   <si>
     <t>0xDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>replica(副本最多5个)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -311,7 +384,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +441,21 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -693,13 +781,109 @@
     <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -711,42 +895,9 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -763,69 +914,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1126,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1236,16 +1324,16 @@
       <c r="B14" s="7">
         <v>1</v>
       </c>
-      <c r="C14" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
+      <c r="C14" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1">
@@ -1255,57 +1343,57 @@
       <c r="B15" s="11">
         <v>2</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="42"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="53"/>
+      <c r="H15" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="52"/>
+      <c r="J15" s="53"/>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="16">
         <v>4</v>
       </c>
-      <c r="C16" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="59"/>
+      <c r="C16" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="44"/>
     </row>
     <row r="17" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="17">
         <v>20</v>
       </c>
-      <c r="C17" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="62"/>
+      <c r="C17" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="10" t="s">
@@ -1314,90 +1402,90 @@
       <c r="B18" s="10">
         <v>25</v>
       </c>
-      <c r="C18" s="64" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="66"/>
+      <c r="C18" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="14">
         <v>29</v>
       </c>
-      <c r="C19" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="72"/>
+      <c r="C19" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="62"/>
     </row>
     <row r="20" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" s="15">
         <v>33</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="69"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="75"/>
+      <c r="D21" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="65"/>
     </row>
     <row r="22" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="39"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="50"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
@@ -1483,16 +1571,16 @@
       <c r="B36" s="7">
         <v>1</v>
       </c>
-      <c r="C36" s="43" t="s">
+      <c r="C36" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="45"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="41"/>
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" ht="20.100000000000001" customHeight="1">
@@ -1502,275 +1590,262 @@
       <c r="B37" s="19">
         <v>2</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="G37" s="49"/>
-      <c r="H37" s="50" t="s">
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="G37" s="70"/>
+      <c r="H37" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="51"/>
-      <c r="J37" s="52"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="73"/>
       <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="48"/>
+      <c r="C38" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="33"/>
       <c r="E38" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="54"/>
+      <c r="G38" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="75"/>
       <c r="K38" s="5"/>
     </row>
     <row r="39" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="48"/>
+      <c r="C39" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="48"/>
+        <v>50</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="48"/>
+      <c r="C41" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="33"/>
     </row>
     <row r="42" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="48"/>
+        <v>50</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="33"/>
     </row>
     <row r="43" spans="1:11" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="33"/>
+        <v>61</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="35"/>
       <c r="E43" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="G43" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="56"/>
+      <c r="G43" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="37"/>
       <c r="K43" s="5"/>
     </row>
     <row r="44" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="33"/>
+        <v>62</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="33"/>
+        <v>50</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="33"/>
+        <v>64</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="35"/>
     </row>
     <row r="47" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="33"/>
+        <v>50</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="35"/>
     </row>
     <row r="48" spans="1:11" s="9" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-      <c r="J48" s="36"/>
+      <c r="C48" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="67"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="68"/>
     </row>
     <row r="49" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C49" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="39"/>
+      <c r="C49" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="C16:J16"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="C19:J19"/>
-    <mergeCell ref="D21:J21"/>
     <mergeCell ref="D45:J45"/>
     <mergeCell ref="D47:J47"/>
     <mergeCell ref="C48:J48"/>
@@ -1787,9 +1862,23 @@
     <mergeCell ref="C41:J41"/>
     <mergeCell ref="D40:J40"/>
     <mergeCell ref="G38:J38"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="C18:J18"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C19:J19"/>
+    <mergeCell ref="D21:J21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>